<commit_message>
added excel helper, keywords and locator helper classes
</commit_message>
<xml_diff>
--- a/resources/input.xlsx
+++ b/resources/input.xlsx
@@ -95,9 +95,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>fillTextFiled</t>
-  </si>
-  <si>
     <t>enter password</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>fillTextField</t>
   </si>
 </sst>
 </file>
@@ -606,15 +606,15 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -630,7 +630,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,19 +716,19 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,16 +736,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -753,13 +753,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>3000</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,16 +767,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -784,16 +784,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -801,19 +801,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -821,19 +821,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>45</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -841,16 +841,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -858,10 +858,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
         <v>49</v>
-      </c>
-      <c r="F13" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -869,27 +869,27 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
         <v>51</v>
-      </c>
-      <c r="F14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>54</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" t="s">
-        <v>56</v>
-      </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete keyword driven framework with Driver class
</commit_message>
<xml_diff>
--- a/resources/input.xlsx
+++ b/resources/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="test cases" sheetId="1" r:id="rId1"/>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>